<commit_message>
add task2 def test_multi and fix(main): def sum
</commit_message>
<xml_diff>
--- a/resources/testing_taks2.xlsx
+++ b/resources/testing_taks2.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="56">
   <si>
     <t xml:space="preserve">name </t>
   </si>
@@ -150,6 +150,45 @@
   </si>
   <si>
     <t>[1,-2,-3]</t>
+  </si>
+  <si>
+    <t>8.А</t>
+  </si>
+  <si>
+    <t>False вместо элемента</t>
+  </si>
+  <si>
+    <t>[1,2, False,4,5]</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>1.B</t>
+  </si>
+  <si>
+    <t>2.B</t>
+  </si>
+  <si>
+    <t>3.B</t>
+  </si>
+  <si>
+    <t>4.B</t>
+  </si>
+  <si>
+    <t>5.B</t>
+  </si>
+  <si>
+    <t>6.B</t>
+  </si>
+  <si>
+    <t>7.B</t>
+  </si>
+  <si>
+    <t>8.B</t>
   </si>
 </sst>
 </file>
@@ -207,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -220,6 +259,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -492,7 +533,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -500,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,6 +678,15 @@
       <c r="G5" s="1">
         <v>-14</v>
       </c>
+      <c r="I5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -730,76 +780,73 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="3">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+    </row>
+    <row r="12" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="4"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
+      <c r="B12" s="4"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="1">
-        <v>6</v>
-      </c>
-      <c r="G13" s="1"/>
-      <c r="I13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>6</v>
+      <c r="F13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" s="1">
         <v>3</v>
@@ -808,28 +855,21 @@
         <v>18</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F14" s="1">
-        <v>9.1199999999999992</v>
-      </c>
-      <c r="G14" s="1"/>
-      <c r="I14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>38</v>
+        <v>6</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C15" s="1">
         <v>3</v>
@@ -838,19 +878,21 @@
         <v>18</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F15" s="1">
-        <v>-15</v>
-      </c>
-      <c r="G15" s="1"/>
+        <v>9.1199999999999992</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>25</v>
+        <v>50</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="C16" s="1">
         <v>3</v>
@@ -859,40 +901,44 @@
         <v>18</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F16" s="1">
         <v>-6</v>
       </c>
-      <c r="G16" s="1"/>
+      <c r="G16" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="3">
-        <v>2</v>
+        <v>51</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="1">
+        <v>3</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="3">
-        <v>1</v>
-      </c>
-      <c r="G17" s="1"/>
+      <c r="E17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" s="1">
+        <v>-6</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C18" s="3">
         <v>2</v>
@@ -900,22 +946,22 @@
       <c r="D18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>27</v>
+      <c r="E18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="3">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C19" s="3">
         <v>2</v>
@@ -924,7 +970,7 @@
         <v>18</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>27</v>
@@ -933,12 +979,57 @@
         <v>27</v>
       </c>
     </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="3">
+        <v>2</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="3">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="I2:K2"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add task2 def test_average and fix(main): def multi
</commit_message>
<xml_diff>
--- a/resources/testing_taks2.xlsx
+++ b/resources/testing_taks2.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="70">
   <si>
     <t xml:space="preserve">name </t>
   </si>
@@ -189,6 +189,48 @@
   </si>
   <si>
     <t>8.B</t>
+  </si>
+  <si>
+    <t>Testing task2 Array def avarage</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Среднее арифметическое</t>
+  </si>
+  <si>
+    <t>1.C</t>
+  </si>
+  <si>
+    <t>2.C</t>
+  </si>
+  <si>
+    <t>3.C</t>
+  </si>
+  <si>
+    <t>4.C</t>
+  </si>
+  <si>
+    <t>5.C</t>
+  </si>
+  <si>
+    <t>6.C</t>
+  </si>
+  <si>
+    <t>7.C</t>
+  </si>
+  <si>
+    <t>8.C</t>
+  </si>
+  <si>
+    <t>ZeroDivisionError</t>
+  </si>
+  <si>
+    <t>9.C</t>
+  </si>
+  <si>
+    <t>["", 1, {1}, "", None]</t>
   </si>
 </sst>
 </file>
@@ -253,14 +295,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -541,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,16 +595,16 @@
     <col min="4" max="4" width="14.28515625" customWidth="1"/>
     <col min="5" max="5" width="25.85546875" customWidth="1"/>
     <col min="6" max="6" width="17.5703125" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="30.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="40.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="4"/>
+      <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -586,11 +628,11 @@
       <c r="G2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -710,6 +752,15 @@
       <c r="G6" s="1">
         <v>6</v>
       </c>
+      <c r="I6" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -804,19 +855,19 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="4"/>
+      <c r="B12" s="6"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -999,7 +1050,7 @@
         <v>27</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1025,11 +1076,248 @@
         <v>46</v>
       </c>
     </row>
+    <row r="23" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="6"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="1">
+        <v>3</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="1">
+        <v>3</v>
+      </c>
+      <c r="G25" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="1">
+        <v>3</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="G26" s="1">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="1">
+        <v>3</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F27" s="1">
+        <v>-3</v>
+      </c>
+      <c r="G27" s="1">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="1">
+        <v>3</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" s="1">
+        <v>1</v>
+      </c>
+      <c r="G28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="3">
+        <v>2</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="3">
+        <v>2</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="3">
+        <v>2</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="3">
+        <v>2</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" s="3">
+        <v>2</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A23:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>